<commit_message>
Decision Tree gecheckt door Jeroen
</commit_message>
<xml_diff>
--- a/docs/DNN performance using different layer architectures.xlsx
+++ b/docs/DNN performance using different layer architectures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeroe\Documents\Minor AI\Project-AI-minor\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6022DA86-8327-4D40-A7CA-B947D92F7B28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080D7676-4D22-47E7-9F63-B42BF8307A60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="9840" xr2:uid="{4B115271-A39A-4C3B-8135-7E0424ED6DDC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>MODELS</t>
   </si>
@@ -68,142 +68,76 @@
     <t>Dropout</t>
   </si>
   <si>
-    <t>0.1 ,  0.1</t>
-  </si>
-  <si>
-    <t>74.70</t>
-  </si>
-  <si>
-    <t>74.82</t>
-  </si>
-  <si>
-    <t>[[581.2 196.8]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [  9.2  30.8]] </t>
-  </si>
-  <si>
     <t>Conmat</t>
   </si>
   <si>
-    <t>0.7585</t>
-  </si>
-  <si>
-    <t>0.7700</t>
-  </si>
-  <si>
-    <t>[[647.  131. ]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [ 14.6  25.4]] </t>
-  </si>
-  <si>
     <t>25, 5</t>
   </si>
   <si>
-    <t>0.1, 0.1</t>
-  </si>
-  <si>
-    <t>82.20</t>
-  </si>
-  <si>
-    <t>83.16</t>
-  </si>
-  <si>
-    <t>0.7333</t>
-  </si>
-  <si>
-    <t>0.6350</t>
-  </si>
-  <si>
     <t>Class weight</t>
   </si>
   <si>
-    <t>[[633.6 144.4]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [ 11.6  28.4]] </t>
-  </si>
-  <si>
-    <t>0.7100</t>
-  </si>
-  <si>
-    <t>0.7622</t>
-  </si>
-  <si>
-    <t>81.44</t>
-  </si>
-  <si>
-    <t>80.92</t>
-  </si>
-  <si>
     <t>* k-fold cross-validation used for all performance estimations</t>
   </si>
   <si>
-    <t>82.54</t>
-  </si>
-  <si>
-    <t>83.54</t>
-  </si>
-  <si>
-    <t>0.7327</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.6300 </t>
-  </si>
-  <si>
-    <t>[[650.  128. ]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [ 14.8  25.2]] </t>
-  </si>
-  <si>
-    <t>81.47</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 82.08</t>
-  </si>
-  <si>
-    <t>0.7579</t>
-  </si>
-  <si>
-    <t>0.6950</t>
-  </si>
-  <si>
-    <t>[[638.6 139.4]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [ 12.2  27.8]] </t>
-  </si>
-  <si>
-    <t>81.66</t>
-  </si>
-  <si>
-    <t>82.16</t>
-  </si>
-  <si>
-    <t>0.7708</t>
-  </si>
-  <si>
-    <t>0.7200</t>
-  </si>
-  <si>
-    <t>[[639.2 138.8]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [ 11.2  28.8]] </t>
-  </si>
-  <si>
     <t>Oversampling</t>
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>balanced_accuracy_manually</t>
+  </si>
+  <si>
+    <t>[[638,6 139,4]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [ 12,2  27,8]] </t>
+  </si>
+  <si>
+    <t>[[639,2 138,8]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [ 11,2  28,8]] </t>
+  </si>
+  <si>
+    <t>[[633,6 144,4]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [ 11,6  28,4]] </t>
+  </si>
+  <si>
+    <t>[[650,  128, ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [ 14,8  25,2]] </t>
+  </si>
+  <si>
+    <t>0,1, 0,1</t>
+  </si>
+  <si>
+    <t>[[647,  131, ]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [ 14,6  25,4]] </t>
+  </si>
+  <si>
+    <t>0,1 ,  0,1</t>
+  </si>
+  <si>
+    <t>[[581,2 196,8]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [  9,2  30,8]] </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -248,7 +182,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -260,6 +194,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -574,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8760839C-2B81-4378-8A04-808D16BB0962}">
-  <dimension ref="B1:L25"/>
+  <dimension ref="B1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="G3" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -587,29 +522,30 @@
     <col min="5" max="6" width="20.6328125" customWidth="1"/>
     <col min="7" max="7" width="17.26953125" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="12.26953125" customWidth="1"/>
-    <col min="10" max="10" width="11.6328125" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="9" max="9" width="29.36328125" customWidth="1"/>
+    <col min="10" max="10" width="17.26953125" customWidth="1"/>
+    <col min="11" max="11" width="11.6328125" customWidth="1"/>
+    <col min="12" max="12" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C3" s="1" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>3</v>
@@ -624,24 +560,27 @@
         <v>2</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="M3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>15</v>
@@ -653,35 +592,41 @@
         <v>50</v>
       </c>
       <c r="G4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K4" t="s">
-        <v>44</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="L5" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="L6" s="6"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="H4" s="3">
+        <v>81.47</v>
+      </c>
+      <c r="I4" s="7">
+        <f>(K4+L4)/2</f>
+        <v>0.72645000000000004</v>
+      </c>
+      <c r="J4">
+        <v>82.08</v>
+      </c>
+      <c r="K4">
+        <v>0.75790000000000002</v>
+      </c>
+      <c r="L4">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="I5" s="7"/>
+      <c r="M5" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="I6" s="7"/>
+      <c r="M6" s="6"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="D7">
         <v>15</v>
@@ -693,78 +638,90 @@
         <v>50</v>
       </c>
       <c r="G7" t="s">
-        <v>54</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="J7" t="s">
-        <v>49</v>
-      </c>
-      <c r="K7" t="s">
-        <v>50</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="L8" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="L9" s="6"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="H7" s="3">
+        <v>81.66</v>
+      </c>
+      <c r="I7" s="7">
+        <f t="shared" ref="I5:I19" si="0">(K7+L7)/2</f>
+        <v>0.74540000000000006</v>
+      </c>
+      <c r="J7" s="3">
+        <v>82.16</v>
+      </c>
+      <c r="K7">
+        <v>0.77080000000000004</v>
+      </c>
+      <c r="L7">
+        <v>0.72</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="I8" s="7"/>
+      <c r="M8" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="I9" s="7"/>
+      <c r="M9" s="6"/>
+    </row>
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="D10">
         <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F10">
         <v>50</v>
       </c>
       <c r="G10" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" t="s">
-        <v>33</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J10" t="s">
-        <v>31</v>
-      </c>
-      <c r="K10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L10" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="L11" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="L12" s="2"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="H10">
+        <v>80.92</v>
+      </c>
+      <c r="I10" s="7">
+        <f t="shared" si="0"/>
+        <v>0.73609999999999998</v>
+      </c>
+      <c r="J10" s="3">
+        <v>81.44</v>
+      </c>
+      <c r="K10">
+        <v>0.76219999999999999</v>
+      </c>
+      <c r="L10">
+        <v>0.71</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="I11" s="7"/>
+      <c r="M11" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="I12" s="7"/>
+      <c r="M12" s="2"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="D13">
         <v>15</v>
@@ -776,75 +733,87 @@
         <v>50</v>
       </c>
       <c r="G13" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="I13" t="s">
-        <v>36</v>
-      </c>
-      <c r="J13" t="s">
-        <v>37</v>
-      </c>
-      <c r="K13" t="s">
-        <v>38</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="L14" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="L15" s="2"/>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+      <c r="H13" s="4">
+        <v>82.54</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" si="0"/>
+        <v>0.68135000000000001</v>
+      </c>
+      <c r="J13">
+        <v>83.54</v>
+      </c>
+      <c r="K13">
+        <v>0.73270000000000002</v>
+      </c>
+      <c r="L13">
+        <v>0.63</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="I14" s="7"/>
+      <c r="M14" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
+      <c r="I15" s="7"/>
+      <c r="M15" s="2"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
       <c r="C16" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="D16">
         <v>15</v>
       </c>
       <c r="E16" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="F16">
         <v>50</v>
       </c>
       <c r="G16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" t="s">
-        <v>23</v>
-      </c>
-      <c r="I16" t="s">
-        <v>24</v>
-      </c>
-      <c r="J16" t="s">
-        <v>25</v>
-      </c>
-      <c r="K16" t="s">
         <v>26</v>
       </c>
-      <c r="L16" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="L17" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="L18" s="2"/>
-    </row>
-    <row r="19" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="H16">
+        <v>82.2</v>
+      </c>
+      <c r="I16" s="7">
+        <f t="shared" si="0"/>
+        <v>0.68415000000000004</v>
+      </c>
+      <c r="J16">
+        <v>83.16</v>
+      </c>
+      <c r="K16">
+        <v>0.73329999999999995</v>
+      </c>
+      <c r="L16">
+        <v>0.63500000000000001</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="I17" s="7"/>
+      <c r="M17" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="I18" s="7"/>
+      <c r="M18" s="2"/>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.35">
       <c r="C19" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="D19">
         <v>15</v>
@@ -856,43 +825,47 @@
         <v>50</v>
       </c>
       <c r="G19" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I19" t="s">
-        <v>12</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K19" t="s">
-        <v>18</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="L20" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="L21" s="2"/>
-    </row>
-    <row r="22" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="L22" s="2"/>
-    </row>
-    <row r="23" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="L23" s="2"/>
-    </row>
-    <row r="24" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="L24" s="2"/>
-    </row>
-    <row r="25" spans="3:12" x14ac:dyDescent="0.35">
-      <c r="L25" s="2"/>
+        <v>29</v>
+      </c>
+      <c r="H19" s="3">
+        <v>74.819999999999993</v>
+      </c>
+      <c r="I19" s="7">
+        <f t="shared" si="0"/>
+        <v>0.76424999999999998</v>
+      </c>
+      <c r="J19">
+        <v>74.7</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0.75849999999999995</v>
+      </c>
+      <c r="L19">
+        <v>0.77</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="M20" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="M21" s="2"/>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="M22" s="2"/>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="M23" s="2"/>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="M24" s="2"/>
+    </row>
+    <row r="25" spans="3:13" x14ac:dyDescent="0.35">
+      <c r="M25" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>